<commit_message>
update the peer review sheet
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Login_Registration_PR.xlsx
+++ b/Car_TestCases/Car_Login_Registration_PR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,48 @@
   </si>
   <si>
     <t xml:space="preserve">not a bug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no related SRS ID's column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no column for the reviewer </t>
+  </si>
+  <si>
+    <t>Car_PR_01</t>
+  </si>
+  <si>
+    <t>Car_PR_ID</t>
+  </si>
+  <si>
+    <t>Car_PR_02</t>
+  </si>
+  <si>
+    <t>Car_PR_03</t>
+  </si>
+  <si>
+    <t>Car_PR_04</t>
+  </si>
+  <si>
+    <t>Car_PR_05</t>
+  </si>
+  <si>
+    <t>Car_PR_06</t>
+  </si>
+  <si>
+    <t>Car_PR_07</t>
+  </si>
+  <si>
+    <t>Car_PR_08</t>
+  </si>
+  <si>
+    <t>Car_PR_09</t>
+  </si>
+  <si>
+    <t>Car_PR_10</t>
+  </si>
+  <si>
+    <t>please try to work on the last version of the project cause there is  new updates</t>
   </si>
 </sst>
 </file>
@@ -464,49 +506,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="2"/>
-    <col min="2" max="2" width="96.5703125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="27.42578125" style="2"/>
+    <col min="1" max="2" width="27.42578125" style="2"/>
+    <col min="3" max="3" width="96.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="27.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3" s="8" customFormat="1" ht="21" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="21" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="21" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>